<commit_message>
working with script 2
</commit_message>
<xml_diff>
--- a/R_output_files/Tables/Cell_Type_Markers_Summary.xlsx
+++ b/R_output_files/Tables/Cell_Type_Markers_Summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,190 +392,240 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dendritic cells</t>
+          <t>Crypt cells</t>
         </is>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Endothelial cells</t>
+          <t>Dendritic cells</t>
         </is>
       </c>
       <c r="B5">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Enterochromaffin cells</t>
+          <t>Endothelial cells</t>
         </is>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Enteroendocrine cells</t>
+          <t>Enterochromaffin cells</t>
         </is>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Eosinophils</t>
+          <t>Enteroendocrine cells</t>
         </is>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Foveolar cells</t>
+          <t>Eosinophils</t>
         </is>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Gastric chief cells</t>
+          <t>Fibroblasts</t>
         </is>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Macrophages</t>
+          <t>Foveolar cells</t>
         </is>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mast cells</t>
+          <t>Gastric chief cells</t>
         </is>
       </c>
       <c r="B12">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Metaplastic cells</t>
+          <t>Macrophages</t>
         </is>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Monocytes</t>
+          <t>Mast cells</t>
         </is>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mucous neck cells</t>
+          <t>Metaplastic cells</t>
         </is>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Natural killer T cells</t>
+          <t>Monocytes</t>
         </is>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Neutrophils</t>
+          <t>Mucous neck cells</t>
         </is>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Parietal cells</t>
+          <t>Natural killer T cells</t>
         </is>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Plasma cells</t>
+          <t>Neutrophils</t>
         </is>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Plasmacytoid dendritic cells</t>
+          <t>Parietal cells</t>
         </is>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Proliferating Tff2+ cells</t>
+          <t>Pericytes</t>
         </is>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Plasma cells</t>
+        </is>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Plasmacytoid dendritic cells</t>
+        </is>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Proliferating Tff2+ cells</t>
+        </is>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Stromal cells</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>T cells</t>
         </is>
       </c>
-      <c r="B22">
+      <c r="B26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Tuft cells</t>
+        </is>
+      </c>
+      <c r="B27">
         <v>6</v>
       </c>
     </row>

</xml_diff>